<commit_message>
Update French config with new strings
and add them to the excel file for translation
</commit_message>
<xml_diff>
--- a/RAMP/src/assets/RAMP Arctic Fox - Strings for translation June 2014 v.2.xlsx
+++ b/RAMP/src/assets/RAMP Arctic Fox - Strings for translation June 2014 v.2.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="287">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="292">
   <si>
     <t>English</t>
   </si>
@@ -895,6 +895,21 @@
   </si>
   <si>
     <t>Zoom slider</t>
+  </si>
+  <si>
+    <t>txtSettings</t>
+  </si>
+  <si>
+    <t>Settings</t>
+  </si>
+  <si>
+    <t>txtSettingsLayerSettings</t>
+  </si>
+  <si>
+    <t>Layer Settings</t>
+  </si>
+  <si>
+    <t>txtSettingsOpacity</t>
   </si>
 </sst>
 </file>
@@ -1075,7 +1090,19 @@
     <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="33">
+  <dxfs count="34">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="3" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -1488,13 +1515,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>151</xdr:row>
+      <xdr:row>150</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>2857500</xdr:colOff>
-      <xdr:row>151</xdr:row>
+      <xdr:row>150</xdr:row>
       <xdr:rowOff>967740</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1530,13 +1557,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>151</xdr:row>
+      <xdr:row>150</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>1190625</xdr:colOff>
-      <xdr:row>151</xdr:row>
+      <xdr:row>150</xdr:row>
       <xdr:rowOff>200025</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1871,10 +1898,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D154"/>
+  <dimension ref="A1:D153"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A142" workbookViewId="0">
-      <selection activeCell="C154" sqref="C154"/>
+    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
+      <selection activeCell="B114" sqref="B114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2854,13 +2881,37 @@
       <c r="C107" s="17"/>
     </row>
     <row r="108" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="C108" s="17"/>
+      <c r="A108" t="s">
+        <v>287</v>
+      </c>
+      <c r="B108" t="s">
+        <v>288</v>
+      </c>
+      <c r="C108" s="17" t="s">
+        <v>276</v>
+      </c>
     </row>
     <row r="109" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="C109" s="17"/>
+      <c r="A109" t="s">
+        <v>289</v>
+      </c>
+      <c r="B109" t="s">
+        <v>290</v>
+      </c>
+      <c r="C109" s="17" t="s">
+        <v>276</v>
+      </c>
     </row>
     <row r="110" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="C110" s="17"/>
+      <c r="A110" t="s">
+        <v>291</v>
+      </c>
+      <c r="B110" t="s">
+        <v>172</v>
+      </c>
+      <c r="C110" s="17" t="s">
+        <v>276</v>
+      </c>
     </row>
     <row r="111" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="C111" s="17"/>
@@ -2907,422 +2958,414 @@
     <row r="125" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="C125" s="17"/>
     </row>
-    <row r="126" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="C126" s="17"/>
-    </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A128" s="25" t="s">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A127" s="25" t="s">
         <v>154</v>
       </c>
-      <c r="B128" s="25"/>
-      <c r="C128" s="25"/>
-      <c r="D128" s="25"/>
+      <c r="B127" s="25"/>
+      <c r="C127" s="25"/>
+      <c r="D127" s="25"/>
+    </row>
+    <row r="129" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A129" t="s">
+        <v>136</v>
+      </c>
+      <c r="B129" t="s">
+        <v>167</v>
+      </c>
+      <c r="C129" s="17" t="s">
+        <v>248</v>
+      </c>
     </row>
     <row r="130" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B130" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C130" s="17" t="s">
-        <v>248</v>
+        <v>249</v>
+      </c>
+      <c r="D130" s="6" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="131" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B131" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C131" s="17" t="s">
-        <v>249</v>
-      </c>
-      <c r="D131" s="6" t="s">
-        <v>155</v>
+        <v>250</v>
       </c>
     </row>
     <row r="132" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B132" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C132" s="17" t="s">
-        <v>250</v>
+        <v>251</v>
+      </c>
+      <c r="D132" s="6" t="s">
+        <v>169</v>
       </c>
     </row>
     <row r="133" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B133" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="C133" s="17" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="D133" s="6" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="134" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B134" t="s">
-        <v>161</v>
-      </c>
-      <c r="C134" s="17" t="s">
-        <v>252</v>
-      </c>
-      <c r="D134" s="6" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.3">
+        <v>163</v>
+      </c>
+      <c r="C134" s="13" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B135" t="s">
-        <v>163</v>
-      </c>
-      <c r="C135" s="13" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="136" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+        <v>162</v>
+      </c>
+      <c r="C135" s="17" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
-        <v>142</v>
+        <v>168</v>
       </c>
       <c r="B136" t="s">
-        <v>162</v>
-      </c>
-      <c r="C136" s="17" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.3">
+        <v>15</v>
+      </c>
+      <c r="C136" s="13" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
-        <v>168</v>
+        <v>143</v>
       </c>
       <c r="B137" t="s">
-        <v>15</v>
-      </c>
-      <c r="C137" s="13" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="138" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+        <v>156</v>
+      </c>
+      <c r="C137" s="19" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B138" t="s">
-        <v>156</v>
-      </c>
-      <c r="C138" s="19" t="s">
-        <v>254</v>
+        <v>157</v>
+      </c>
+      <c r="C138" s="22" t="s">
+        <v>192</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B139" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C139" s="22" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B140" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="C140" s="22" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B141" t="s">
-        <v>159</v>
+        <v>133</v>
       </c>
       <c r="C141" s="22" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B142" t="s">
-        <v>133</v>
-      </c>
-      <c r="C142" s="22" t="s">
-        <v>195</v>
+        <v>114</v>
+      </c>
+      <c r="C142" s="16" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B143" t="s">
-        <v>114</v>
-      </c>
-      <c r="C143" s="16" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.3">
+        <v>152</v>
+      </c>
+      <c r="C143" s="13" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B144" t="s">
-        <v>152</v>
-      </c>
-      <c r="C144" s="13" t="s">
-        <v>152</v>
+        <v>160</v>
+      </c>
+      <c r="C144" s="17" t="s">
+        <v>255</v>
       </c>
     </row>
     <row r="145" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B145" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="C145" s="17" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="146" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A146" t="s">
-        <v>151</v>
-      </c>
-      <c r="B146" t="s">
-        <v>153</v>
-      </c>
-      <c r="C146" s="17" t="s">
         <v>256</v>
       </c>
     </row>
+    <row r="147" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A147" s="25" t="s">
+        <v>177</v>
+      </c>
+      <c r="B147" s="25"/>
+      <c r="C147" s="25"/>
+      <c r="D147" s="25"/>
+    </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A148" s="25" t="s">
-        <v>177</v>
-      </c>
-      <c r="B148" s="25"/>
-      <c r="C148" s="25"/>
-      <c r="D148" s="25"/>
-    </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A149" s="2"/>
-      <c r="B149" s="2"/>
-      <c r="C149" s="11"/>
-      <c r="D149" s="2"/>
-    </row>
-    <row r="150" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B150" s="9" t="s">
+      <c r="A148" s="2"/>
+      <c r="B148" s="2"/>
+      <c r="C148" s="11"/>
+      <c r="D148" s="2"/>
+    </row>
+    <row r="149" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B149" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="C150" s="17" t="s">
+      <c r="C149" s="17" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="151" spans="1:4" ht="124.8" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:4" ht="124.8" x14ac:dyDescent="0.3">
+      <c r="B150" s="10" t="s">
+        <v>178</v>
+      </c>
+      <c r="C150" s="20" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4" ht="109.2" x14ac:dyDescent="0.3">
       <c r="B151" s="10" t="s">
-        <v>178</v>
-      </c>
-      <c r="C151" s="20" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="152" spans="1:4" ht="109.2" x14ac:dyDescent="0.3">
-      <c r="B152" s="10" t="s">
         <v>179</v>
       </c>
-      <c r="C152" s="21" t="s">
+      <c r="C151" s="21" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B154" t="s">
+    <row r="153" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B153" t="s">
         <v>286</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="A4:D4"/>
-    <mergeCell ref="A128:D128"/>
-    <mergeCell ref="A148:D148"/>
+    <mergeCell ref="A127:D127"/>
+    <mergeCell ref="A147:D147"/>
     <mergeCell ref="A19:D19"/>
     <mergeCell ref="A63:D63"/>
   </mergeCells>
   <conditionalFormatting sqref="A1:D3 A19 A63 A18:D18 A20:D20 A61:D62 A21:B60 D21:D60 A64:D64 A65:B66 D65:D66 C66:C67 C87 C71 C81:C84 C73 C75">
-    <cfRule type="beginsWith" dxfId="32" priority="37" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="31" priority="37" operator="beginsWith" text="#">
       <formula>LEFT(A1,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4:A17">
-    <cfRule type="beginsWith" dxfId="31" priority="36" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="30" priority="36" operator="beginsWith" text="#">
       <formula>LEFT(A4,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C9">
-    <cfRule type="beginsWith" dxfId="30" priority="35" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="29" priority="35" operator="beginsWith" text="#">
       <formula>LEFT(C9,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C23 C25:C26 C30:C41 C56:C60">
-    <cfRule type="beginsWith" dxfId="29" priority="34" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="28" priority="34" operator="beginsWith" text="#">
       <formula>LEFT(C23,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A128">
-    <cfRule type="beginsWith" dxfId="28" priority="33" operator="beginsWith" text="#">
-      <formula>LEFT(A128,LEN("#"))="#"</formula>
+  <conditionalFormatting sqref="A127">
+    <cfRule type="beginsWith" dxfId="27" priority="33" operator="beginsWith" text="#">
+      <formula>LEFT(A127,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C135 C144 C137 C139:C141">
-    <cfRule type="beginsWith" dxfId="27" priority="31" operator="beginsWith" text="#">
-      <formula>LEFT(C135,LEN("#"))="#"</formula>
+  <conditionalFormatting sqref="C134 C143 C136 C138:C140">
+    <cfRule type="beginsWith" dxfId="26" priority="31" operator="beginsWith" text="#">
+      <formula>LEFT(C134,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A148:A149">
-    <cfRule type="beginsWith" dxfId="26" priority="30" operator="beginsWith" text="#">
-      <formula>LEFT(A148,LEN("#"))="#"</formula>
+  <conditionalFormatting sqref="A147:A148">
+    <cfRule type="beginsWith" dxfId="25" priority="30" operator="beginsWith" text="#">
+      <formula>LEFT(A147,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C86">
-    <cfRule type="beginsWith" dxfId="25" priority="28" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="24" priority="28" operator="beginsWith" text="#">
       <formula>LEFT(C86,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C6:C8 C76:C79 C94">
-    <cfRule type="expression" dxfId="24" priority="26" stopIfTrue="1">
+  <conditionalFormatting sqref="C6:C8 C76:C79 C94 C101:C125">
+    <cfRule type="expression" dxfId="23" priority="26" stopIfTrue="1">
       <formula>LEFT(C6,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C10:C12">
-    <cfRule type="expression" dxfId="23" priority="25" stopIfTrue="1">
+    <cfRule type="expression" dxfId="22" priority="25" stopIfTrue="1">
       <formula>LEFT(C10,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C14:C17">
-    <cfRule type="expression" dxfId="22" priority="24" stopIfTrue="1">
+    <cfRule type="expression" dxfId="21" priority="24" stopIfTrue="1">
       <formula>LEFT(C14,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C21:C22">
-    <cfRule type="expression" dxfId="21" priority="23" stopIfTrue="1">
+    <cfRule type="expression" dxfId="20" priority="23" stopIfTrue="1">
       <formula>LEFT(C21,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C24">
-    <cfRule type="expression" dxfId="20" priority="22" stopIfTrue="1">
+    <cfRule type="expression" dxfId="19" priority="22" stopIfTrue="1">
       <formula>LEFT(C24,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C27:C29">
-    <cfRule type="expression" dxfId="19" priority="21" stopIfTrue="1">
+    <cfRule type="expression" dxfId="18" priority="21" stopIfTrue="1">
       <formula>LEFT(C27,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C42:C55">
-    <cfRule type="expression" dxfId="18" priority="20" stopIfTrue="1">
+    <cfRule type="expression" dxfId="17" priority="20" stopIfTrue="1">
       <formula>LEFT(C42,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C65">
-    <cfRule type="expression" dxfId="17" priority="19" stopIfTrue="1">
+    <cfRule type="expression" dxfId="16" priority="19" stopIfTrue="1">
       <formula>LEFT(C65,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C72">
-    <cfRule type="expression" dxfId="16" priority="18" stopIfTrue="1">
+    <cfRule type="expression" dxfId="15" priority="18" stopIfTrue="1">
       <formula>LEFT(C72,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C74">
-    <cfRule type="expression" dxfId="15" priority="17" stopIfTrue="1">
+    <cfRule type="expression" dxfId="14" priority="17" stopIfTrue="1">
       <formula>LEFT(C74,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C85">
-    <cfRule type="expression" dxfId="14" priority="15" stopIfTrue="1">
+    <cfRule type="expression" dxfId="13" priority="15" stopIfTrue="1">
       <formula>LEFT(C85,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C88:C92 C97">
-    <cfRule type="expression" dxfId="13" priority="14" stopIfTrue="1">
+    <cfRule type="expression" dxfId="12" priority="14" stopIfTrue="1">
       <formula>LEFT(C88,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C130:C134">
-    <cfRule type="expression" dxfId="12" priority="13" stopIfTrue="1">
-      <formula>LEFT(C130,LEN("#"))="#"</formula>
+  <conditionalFormatting sqref="C129:C133">
+    <cfRule type="expression" dxfId="11" priority="13" stopIfTrue="1">
+      <formula>LEFT(C129,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C136">
-    <cfRule type="expression" dxfId="11" priority="12" stopIfTrue="1">
-      <formula>LEFT(C136,LEN("#"))="#"</formula>
+  <conditionalFormatting sqref="C135">
+    <cfRule type="expression" dxfId="10" priority="12" stopIfTrue="1">
+      <formula>LEFT(C135,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C138">
-    <cfRule type="expression" dxfId="10" priority="11" stopIfTrue="1">
-      <formula>LEFT(C138,LEN("#"))="#"</formula>
+  <conditionalFormatting sqref="C137">
+    <cfRule type="expression" dxfId="9" priority="11" stopIfTrue="1">
+      <formula>LEFT(C137,LEN("#"))="#"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C144">
+    <cfRule type="expression" dxfId="8" priority="10" stopIfTrue="1">
+      <formula>LEFT(C144,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C145">
-    <cfRule type="expression" dxfId="9" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="7" priority="9" stopIfTrue="1">
       <formula>LEFT(C145,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C146">
-    <cfRule type="expression" dxfId="8" priority="9" stopIfTrue="1">
-      <formula>LEFT(C146,LEN("#"))="#"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C150:C152">
-    <cfRule type="expression" dxfId="7" priority="8" stopIfTrue="1">
-      <formula>LEFT(C150,LEN("#"))="#"</formula>
+  <conditionalFormatting sqref="C149:C151">
+    <cfRule type="expression" dxfId="6" priority="8" stopIfTrue="1">
+      <formula>LEFT(C149,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C95">
-    <cfRule type="expression" dxfId="6" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="5" priority="7" stopIfTrue="1">
       <formula>LEFT(C95,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C96">
-    <cfRule type="expression" dxfId="5" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="4" priority="6" stopIfTrue="1">
       <formula>LEFT(C96,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C98">
-    <cfRule type="expression" dxfId="4" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="3" priority="5" stopIfTrue="1">
       <formula>LEFT(C98,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C99">
-    <cfRule type="expression" dxfId="3" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="2" priority="4" stopIfTrue="1">
       <formula>LEFT(C99,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C100">
-    <cfRule type="expression" dxfId="2" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="1" priority="3" stopIfTrue="1">
       <formula>LEFT(C100,LEN("#"))="#"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C101:C126">
-    <cfRule type="expression" dxfId="1" priority="2" stopIfTrue="1">
-      <formula>LEFT(C101,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C93">
@@ -3337,25 +3380,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement>
-    <Document_x0020_Subject xmlns="6c14b9a8-0cf3-4383-834f-1018380d8abf">Detailed Design</Document_x0020_Subject>
-    <_Status xmlns="http://schemas.microsoft.com/sharepoint/v3/fields">Not Started</_Status>
-    <Document_x0020_Category xmlns="6c14b9a8-0cf3-4383-834f-1018380d8abf">Development</Document_x0020_Category>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A328EC7CAE967C42BF4B34D61A06A4B5" ma:contentTypeVersion="6" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="edcd34646fceb0c4bcc9308538c5ed43">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="http://schemas.microsoft.com/sharepoint/v3/fields" xmlns:ns3="6c14b9a8-0cf3-4383-834f-1018380d8abf" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9deb4a6428fe92bbf1d3db187a263d42" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3/fields"/>
@@ -3470,31 +3494,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A766AC35-CC0B-4B7E-9290-4E442146633E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/fields"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="6c14b9a8-0cf3-4383-834f-1018380d8abf"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8B70E11A-8654-45A3-8334-FE029118DA1A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement>
+    <Document_x0020_Subject xmlns="6c14b9a8-0cf3-4383-834f-1018380d8abf">Detailed Design</Document_x0020_Subject>
+    <_Status xmlns="http://schemas.microsoft.com/sharepoint/v3/fields">Not Started</_Status>
+    <Document_x0020_Category xmlns="6c14b9a8-0cf3-4383-834f-1018380d8abf">Development</Document_x0020_Category>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4D694661-529E-46DF-82AC-97A5D29D95C8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3510,4 +3529,28 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/internal/2005/internalDocumentation"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8B70E11A-8654-45A3-8334-FE029118DA1A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A766AC35-CC0B-4B7E-9290-4E442146633E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/fields"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="6c14b9a8-0cf3-4383-834f-1018380d8abf"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Fix missing pagination string; Fix mixed up sort up/down strings;
</commit_message>
<xml_diff>
--- a/RAMP/src/assets/RAMP Arctic Fox - Strings for translation June 2014 v.2.xlsx
+++ b/RAMP/src/assets/RAMP Arctic Fox - Strings for translation June 2014 v.2.xlsx
@@ -1090,31 +1090,7 @@
     <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="34">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="32">
     <dxf>
       <font>
         <b/>
@@ -1900,8 +1876,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D153"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="B114" sqref="B114"/>
+    <sheetView tabSelected="1" topLeftCell="A133" workbookViewId="0">
+      <selection activeCell="D144" sqref="D144"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3148,7 +3124,7 @@
         <v>160</v>
       </c>
       <c r="C144" s="17" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
     </row>
     <row r="145" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
@@ -3159,7 +3135,7 @@
         <v>153</v>
       </c>
       <c r="C145" s="17" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.3">
@@ -3328,14 +3304,14 @@
       <formula>LEFT(C137,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C144">
+  <conditionalFormatting sqref="C145">
     <cfRule type="expression" dxfId="8" priority="10" stopIfTrue="1">
-      <formula>LEFT(C144,LEN("#"))="#"</formula>
+      <formula>LEFT(C145,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C145">
+  <conditionalFormatting sqref="C144">
     <cfRule type="expression" dxfId="7" priority="9" stopIfTrue="1">
-      <formula>LEFT(C145,LEN("#"))="#"</formula>
+      <formula>LEFT(C144,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C149:C151">
@@ -3380,6 +3356,25 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement>
+    <Document_x0020_Subject xmlns="6c14b9a8-0cf3-4383-834f-1018380d8abf">Detailed Design</Document_x0020_Subject>
+    <_Status xmlns="http://schemas.microsoft.com/sharepoint/v3/fields">Not Started</_Status>
+    <Document_x0020_Category xmlns="6c14b9a8-0cf3-4383-834f-1018380d8abf">Development</Document_x0020_Category>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A328EC7CAE967C42BF4B34D61A06A4B5" ma:contentTypeVersion="6" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="edcd34646fceb0c4bcc9308538c5ed43">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="http://schemas.microsoft.com/sharepoint/v3/fields" xmlns:ns3="6c14b9a8-0cf3-4383-834f-1018380d8abf" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9deb4a6428fe92bbf1d3db187a263d42" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3/fields"/>
@@ -3494,26 +3489,31 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A766AC35-CC0B-4B7E-9290-4E442146633E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/fields"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="6c14b9a8-0cf3-4383-834f-1018380d8abf"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement>
-    <Document_x0020_Subject xmlns="6c14b9a8-0cf3-4383-834f-1018380d8abf">Detailed Design</Document_x0020_Subject>
-    <_Status xmlns="http://schemas.microsoft.com/sharepoint/v3/fields">Not Started</_Status>
-    <Document_x0020_Category xmlns="6c14b9a8-0cf3-4383-834f-1018380d8abf">Development</Document_x0020_Category>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8B70E11A-8654-45A3-8334-FE029118DA1A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4D694661-529E-46DF-82AC-97A5D29D95C8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3529,28 +3529,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/internal/2005/internalDocumentation"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8B70E11A-8654-45A3-8334-FE029118DA1A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A766AC35-CC0B-4B7E-9290-4E442146633E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/fields"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="6c14b9a8-0cf3-4383-834f-1018380d8abf"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Update strings for translation list
</commit_message>
<xml_diff>
--- a/RAMP/src/assets/RAMP Arctic Fox - Strings for translation June 2014 v.2.xlsx
+++ b/RAMP/src/assets/RAMP Arctic Fox - Strings for translation June 2014 v.2.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="292">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="316">
   <si>
     <t>English</t>
   </si>
@@ -910,6 +910,78 @@
   </si>
   <si>
     <t>txtSettingsOpacity</t>
+  </si>
+  <si>
+    <t>Loade</t>
+  </si>
+  <si>
+    <t>txtGetLinkShort</t>
+  </si>
+  <si>
+    <t>Short link</t>
+  </si>
+  <si>
+    <t>txtGetLinkLong</t>
+  </si>
+  <si>
+    <t>Long link</t>
+  </si>
+  <si>
+    <t>txtLegend</t>
+  </si>
+  <si>
+    <t>Legend</t>
+  </si>
+  <si>
+    <t>txtLinkToCap</t>
+  </si>
+  <si>
+    <t>Link To Capabilities</t>
+  </si>
+  <si>
+    <t>txtBaseToolClearMap</t>
+  </si>
+  <si>
+    <t>Clear</t>
+  </si>
+  <si>
+    <t>txtBaseToolWorking</t>
+  </si>
+  <si>
+    <t>Working ...</t>
+  </si>
+  <si>
+    <t>txtBufferToolDistance</t>
+  </si>
+  <si>
+    <t>Distance</t>
+  </si>
+  <si>
+    <t>txtMeasureToolLength</t>
+  </si>
+  <si>
+    <t>Length</t>
+  </si>
+  <si>
+    <t>txtMeasureToolArea</t>
+  </si>
+  <si>
+    <t>Area</t>
+  </si>
+  <si>
+    <t>txtMeasureToolNA</t>
+  </si>
+  <si>
+    <t>n/a</t>
+  </si>
+  <si>
+    <t>txtPopulationToolPopulation</t>
+  </si>
+  <si>
+    <t>Population</t>
+  </si>
+  <si>
+    <t>txtPopulationToolNA</t>
   </si>
 </sst>
 </file>
@@ -1090,7 +1162,79 @@
     <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="32">
+  <dxfs count="38">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="3" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="3" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="3" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="3" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="3" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="3" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -1491,13 +1635,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>150</xdr:row>
+      <xdr:row>158</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>2857500</xdr:colOff>
-      <xdr:row>150</xdr:row>
+      <xdr:row>158</xdr:row>
       <xdr:rowOff>967740</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1533,13 +1677,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>150</xdr:row>
+      <xdr:row>158</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>1190625</xdr:colOff>
-      <xdr:row>150</xdr:row>
+      <xdr:row>158</xdr:row>
       <xdr:rowOff>200025</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1874,17 +2018,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D153"/>
+  <dimension ref="A1:D161"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A133" workbookViewId="0">
-      <selection activeCell="D144" sqref="D144"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="C116" sqref="C116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="31" customWidth="1"/>
     <col min="2" max="2" width="63.88671875" customWidth="1"/>
-    <col min="3" max="3" width="37.6640625" style="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="48.77734375" style="12" customWidth="1"/>
     <col min="4" max="4" width="56" style="6" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2857,22 +3001,14 @@
       <c r="C107" s="17"/>
     </row>
     <row r="108" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A108" t="s">
-        <v>287</v>
-      </c>
-      <c r="B108" t="s">
-        <v>288</v>
-      </c>
-      <c r="C108" s="17" t="s">
-        <v>276</v>
-      </c>
+      <c r="C108" s="17"/>
     </row>
     <row r="109" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
-        <v>289</v>
+        <v>279</v>
       </c>
       <c r="B109" t="s">
-        <v>290</v>
+        <v>281</v>
       </c>
       <c r="C109" s="17" t="s">
         <v>276</v>
@@ -2880,472 +3016,632 @@
     </row>
     <row r="110" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
-        <v>291</v>
+        <v>280</v>
       </c>
       <c r="B110" t="s">
-        <v>172</v>
+        <v>282</v>
       </c>
       <c r="C110" s="17" t="s">
         <v>276</v>
       </c>
     </row>
     <row r="111" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="C111" s="17"/>
+      <c r="A111" t="s">
+        <v>277</v>
+      </c>
+      <c r="B111" t="s">
+        <v>283</v>
+      </c>
+      <c r="C111" s="17" t="s">
+        <v>276</v>
+      </c>
     </row>
     <row r="112" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="C112" s="17"/>
-    </row>
-    <row r="113" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A112" t="s">
+        <v>278</v>
+      </c>
+      <c r="B112" t="s">
+        <v>292</v>
+      </c>
+      <c r="C112" s="17" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="C113" s="17"/>
     </row>
-    <row r="114" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="C114" s="17"/>
-    </row>
-    <row r="115" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="C115" s="17"/>
-    </row>
-    <row r="116" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="C116" s="17"/>
-    </row>
-    <row r="117" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="C117" s="17"/>
-    </row>
-    <row r="118" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="C118" s="17"/>
-    </row>
-    <row r="119" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A114" t="s">
+        <v>287</v>
+      </c>
+      <c r="B114" t="s">
+        <v>288</v>
+      </c>
+      <c r="C114" s="17" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A115" t="s">
+        <v>289</v>
+      </c>
+      <c r="B115" t="s">
+        <v>290</v>
+      </c>
+      <c r="C115" s="17" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A116" t="s">
+        <v>291</v>
+      </c>
+      <c r="B116" t="s">
+        <v>172</v>
+      </c>
+      <c r="C116" s="17" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A117" t="s">
+        <v>293</v>
+      </c>
+      <c r="B117" t="s">
+        <v>294</v>
+      </c>
+      <c r="C117" s="17" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A118" t="s">
+        <v>295</v>
+      </c>
+      <c r="B118" t="s">
+        <v>296</v>
+      </c>
+      <c r="C118" s="17" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="C119" s="17"/>
     </row>
-    <row r="120" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="C120" s="17"/>
-    </row>
-    <row r="121" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="C121" s="17"/>
-    </row>
-    <row r="122" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="C122" s="17"/>
-    </row>
-    <row r="123" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="C123" s="17"/>
-    </row>
-    <row r="124" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="C124" s="17"/>
-    </row>
-    <row r="125" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="C125" s="17"/>
-    </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A127" s="25" t="s">
-        <v>154</v>
-      </c>
-      <c r="B127" s="25"/>
-      <c r="C127" s="25"/>
-      <c r="D127" s="25"/>
+    <row r="120" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A120" t="s">
+        <v>297</v>
+      </c>
+      <c r="B120" t="s">
+        <v>298</v>
+      </c>
+      <c r="C120" s="17" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A121" t="s">
+        <v>299</v>
+      </c>
+      <c r="B121" t="s">
+        <v>300</v>
+      </c>
+      <c r="C121" s="17" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A122" t="s">
+        <v>301</v>
+      </c>
+      <c r="B122" t="s">
+        <v>302</v>
+      </c>
+      <c r="C122" s="17" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A123" t="s">
+        <v>303</v>
+      </c>
+      <c r="B123" t="s">
+        <v>304</v>
+      </c>
+      <c r="C123" s="17" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A124" t="s">
+        <v>305</v>
+      </c>
+      <c r="B124" t="s">
+        <v>306</v>
+      </c>
+      <c r="C124" s="17" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A125" t="s">
+        <v>307</v>
+      </c>
+      <c r="B125" t="s">
+        <v>308</v>
+      </c>
+      <c r="C125" s="17" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A126" t="s">
+        <v>309</v>
+      </c>
+      <c r="B126" t="s">
+        <v>310</v>
+      </c>
+      <c r="C126" s="17" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A127" t="s">
+        <v>311</v>
+      </c>
+      <c r="B127" t="s">
+        <v>312</v>
+      </c>
+      <c r="C127" s="17" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A128" t="s">
+        <v>313</v>
+      </c>
+      <c r="B128" t="s">
+        <v>314</v>
+      </c>
+      <c r="C128" s="17" t="s">
+        <v>276</v>
+      </c>
     </row>
     <row r="129" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
-        <v>136</v>
+        <v>315</v>
       </c>
       <c r="B129" t="s">
-        <v>167</v>
+        <v>312</v>
       </c>
       <c r="C129" s="17" t="s">
-        <v>248</v>
+        <v>276</v>
       </c>
     </row>
     <row r="130" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A130" t="s">
-        <v>137</v>
-      </c>
-      <c r="B130" t="s">
-        <v>166</v>
-      </c>
-      <c r="C130" s="17" t="s">
-        <v>249</v>
-      </c>
-      <c r="D130" s="6" t="s">
-        <v>155</v>
-      </c>
+      <c r="C130" s="17"/>
     </row>
     <row r="131" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A131" t="s">
-        <v>138</v>
-      </c>
-      <c r="B131" t="s">
-        <v>165</v>
-      </c>
-      <c r="C131" s="17" t="s">
-        <v>250</v>
-      </c>
+      <c r="C131" s="17"/>
     </row>
     <row r="132" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A132" t="s">
-        <v>139</v>
-      </c>
-      <c r="B132" t="s">
-        <v>164</v>
-      </c>
-      <c r="C132" s="17" t="s">
-        <v>251</v>
-      </c>
-      <c r="D132" s="6" t="s">
-        <v>169</v>
-      </c>
+      <c r="C132" s="17"/>
     </row>
     <row r="133" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A133" t="s">
-        <v>140</v>
-      </c>
-      <c r="B133" t="s">
-        <v>161</v>
-      </c>
-      <c r="C133" s="17" t="s">
-        <v>252</v>
-      </c>
-      <c r="D133" s="6" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A134" t="s">
-        <v>141</v>
-      </c>
-      <c r="B134" t="s">
-        <v>163</v>
-      </c>
-      <c r="C134" s="13" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="135" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A135" t="s">
-        <v>142</v>
-      </c>
-      <c r="B135" t="s">
-        <v>162</v>
-      </c>
-      <c r="C135" s="17" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A136" t="s">
-        <v>168</v>
-      </c>
-      <c r="B136" t="s">
-        <v>15</v>
-      </c>
-      <c r="C136" s="13" t="s">
-        <v>205</v>
-      </c>
+      <c r="C133" s="17"/>
+    </row>
+    <row r="135" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A135" s="25" t="s">
+        <v>154</v>
+      </c>
+      <c r="B135" s="25"/>
+      <c r="C135" s="25"/>
+      <c r="D135" s="25"/>
     </row>
     <row r="137" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="B137" t="s">
-        <v>156</v>
-      </c>
-      <c r="C137" s="19" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.3">
+        <v>167</v>
+      </c>
+      <c r="C137" s="17" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="B138" t="s">
-        <v>157</v>
-      </c>
-      <c r="C138" s="22" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.3">
+        <v>166</v>
+      </c>
+      <c r="C138" s="17" t="s">
+        <v>249</v>
+      </c>
+      <c r="D138" s="6" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="B139" t="s">
-        <v>158</v>
-      </c>
-      <c r="C139" s="22" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.3">
+        <v>165</v>
+      </c>
+      <c r="C139" s="17" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="B140" t="s">
-        <v>159</v>
-      </c>
-      <c r="C140" s="22" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.3">
+        <v>164</v>
+      </c>
+      <c r="C140" s="17" t="s">
+        <v>251</v>
+      </c>
+      <c r="D140" s="6" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="B141" t="s">
-        <v>133</v>
-      </c>
-      <c r="C141" s="22" t="s">
-        <v>195</v>
+        <v>161</v>
+      </c>
+      <c r="C141" s="17" t="s">
+        <v>252</v>
+      </c>
+      <c r="D141" s="6" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="B142" t="s">
-        <v>114</v>
-      </c>
-      <c r="C142" s="16" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.3">
+        <v>163</v>
+      </c>
+      <c r="C142" s="13" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="B143" t="s">
-        <v>152</v>
-      </c>
-      <c r="C143" s="13" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="144" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+        <v>162</v>
+      </c>
+      <c r="C143" s="17" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
-        <v>150</v>
+        <v>168</v>
       </c>
       <c r="B144" t="s">
-        <v>160</v>
-      </c>
-      <c r="C144" s="17" t="s">
-        <v>256</v>
+        <v>15</v>
+      </c>
+      <c r="C144" s="13" t="s">
+        <v>205</v>
       </c>
     </row>
     <row r="145" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
+        <v>143</v>
+      </c>
+      <c r="B145" t="s">
+        <v>156</v>
+      </c>
+      <c r="C145" s="19" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A146" t="s">
+        <v>144</v>
+      </c>
+      <c r="B146" t="s">
+        <v>157</v>
+      </c>
+      <c r="C146" s="22" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A147" t="s">
+        <v>145</v>
+      </c>
+      <c r="B147" t="s">
+        <v>158</v>
+      </c>
+      <c r="C147" s="22" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A148" t="s">
+        <v>146</v>
+      </c>
+      <c r="B148" t="s">
+        <v>159</v>
+      </c>
+      <c r="C148" s="22" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A149" t="s">
+        <v>147</v>
+      </c>
+      <c r="B149" t="s">
+        <v>133</v>
+      </c>
+      <c r="C149" s="22" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A150" t="s">
+        <v>148</v>
+      </c>
+      <c r="B150" t="s">
+        <v>114</v>
+      </c>
+      <c r="C150" s="16" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A151" t="s">
+        <v>149</v>
+      </c>
+      <c r="B151" t="s">
+        <v>152</v>
+      </c>
+      <c r="C151" s="13" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A152" t="s">
+        <v>150</v>
+      </c>
+      <c r="B152" t="s">
+        <v>160</v>
+      </c>
+      <c r="C152" s="17" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="153" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A153" t="s">
         <v>151</v>
       </c>
-      <c r="B145" t="s">
+      <c r="B153" t="s">
         <v>153</v>
       </c>
-      <c r="C145" s="17" t="s">
+      <c r="C153" s="17" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A147" s="25" t="s">
+    <row r="155" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A155" s="25" t="s">
         <v>177</v>
       </c>
-      <c r="B147" s="25"/>
-      <c r="C147" s="25"/>
-      <c r="D147" s="25"/>
-    </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A148" s="2"/>
-      <c r="B148" s="2"/>
-      <c r="C148" s="11"/>
-      <c r="D148" s="2"/>
-    </row>
-    <row r="149" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B149" s="9" t="s">
+      <c r="B155" s="25"/>
+      <c r="C155" s="25"/>
+      <c r="D155" s="25"/>
+    </row>
+    <row r="156" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A156" s="2"/>
+      <c r="B156" s="2"/>
+      <c r="C156" s="11"/>
+      <c r="D156" s="2"/>
+    </row>
+    <row r="157" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B157" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="C149" s="17" t="s">
+      <c r="C157" s="17" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="150" spans="1:4" ht="124.8" x14ac:dyDescent="0.3">
-      <c r="B150" s="10" t="s">
+    <row r="158" spans="1:4" ht="124.8" x14ac:dyDescent="0.3">
+      <c r="B158" s="10" t="s">
         <v>178</v>
       </c>
-      <c r="C150" s="20" t="s">
+      <c r="C158" s="20" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="151" spans="1:4" ht="109.2" x14ac:dyDescent="0.3">
-      <c r="B151" s="10" t="s">
+    <row r="159" spans="1:4" ht="109.2" x14ac:dyDescent="0.3">
+      <c r="B159" s="10" t="s">
         <v>179</v>
       </c>
-      <c r="C151" s="21" t="s">
+      <c r="C159" s="21" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B153" t="s">
+    <row r="161" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B161" t="s">
         <v>286</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="A4:D4"/>
-    <mergeCell ref="A127:D127"/>
-    <mergeCell ref="A147:D147"/>
+    <mergeCell ref="A135:D135"/>
+    <mergeCell ref="A155:D155"/>
     <mergeCell ref="A19:D19"/>
     <mergeCell ref="A63:D63"/>
   </mergeCells>
   <conditionalFormatting sqref="A1:D3 A19 A63 A18:D18 A20:D20 A61:D62 A21:B60 D21:D60 A64:D64 A65:B66 D65:D66 C66:C67 C87 C71 C81:C84 C73 C75">
-    <cfRule type="beginsWith" dxfId="31" priority="37" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="37" priority="37" operator="beginsWith" text="#">
       <formula>LEFT(A1,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4:A17">
-    <cfRule type="beginsWith" dxfId="30" priority="36" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="36" priority="36" operator="beginsWith" text="#">
       <formula>LEFT(A4,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C9">
-    <cfRule type="beginsWith" dxfId="29" priority="35" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="35" priority="35" operator="beginsWith" text="#">
       <formula>LEFT(C9,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C23 C25:C26 C30:C41 C56:C60">
-    <cfRule type="beginsWith" dxfId="28" priority="34" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="34" priority="34" operator="beginsWith" text="#">
       <formula>LEFT(C23,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A127">
-    <cfRule type="beginsWith" dxfId="27" priority="33" operator="beginsWith" text="#">
-      <formula>LEFT(A127,LEN("#"))="#"</formula>
+  <conditionalFormatting sqref="A135">
+    <cfRule type="beginsWith" dxfId="33" priority="33" operator="beginsWith" text="#">
+      <formula>LEFT(A135,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C134 C143 C136 C138:C140">
-    <cfRule type="beginsWith" dxfId="26" priority="31" operator="beginsWith" text="#">
-      <formula>LEFT(C134,LEN("#"))="#"</formula>
+  <conditionalFormatting sqref="C142 C151 C144 C146:C148">
+    <cfRule type="beginsWith" dxfId="32" priority="31" operator="beginsWith" text="#">
+      <formula>LEFT(C142,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A147:A148">
-    <cfRule type="beginsWith" dxfId="25" priority="30" operator="beginsWith" text="#">
-      <formula>LEFT(A147,LEN("#"))="#"</formula>
+  <conditionalFormatting sqref="A155:A156">
+    <cfRule type="beginsWith" dxfId="31" priority="30" operator="beginsWith" text="#">
+      <formula>LEFT(A155,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C86">
-    <cfRule type="beginsWith" dxfId="24" priority="28" operator="beginsWith" text="#">
+    <cfRule type="beginsWith" dxfId="30" priority="28" operator="beginsWith" text="#">
       <formula>LEFT(C86,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C6:C8 C76:C79 C94 C101:C125">
-    <cfRule type="expression" dxfId="23" priority="26" stopIfTrue="1">
+  <conditionalFormatting sqref="C6:C8 C76:C79 C94 C101:C133">
+    <cfRule type="expression" dxfId="29" priority="26" stopIfTrue="1">
       <formula>LEFT(C6,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C10:C12">
-    <cfRule type="expression" dxfId="22" priority="25" stopIfTrue="1">
+    <cfRule type="expression" dxfId="28" priority="25" stopIfTrue="1">
       <formula>LEFT(C10,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C14:C17">
-    <cfRule type="expression" dxfId="21" priority="24" stopIfTrue="1">
+    <cfRule type="expression" dxfId="27" priority="24" stopIfTrue="1">
       <formula>LEFT(C14,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C21:C22">
-    <cfRule type="expression" dxfId="20" priority="23" stopIfTrue="1">
+    <cfRule type="expression" dxfId="26" priority="23" stopIfTrue="1">
       <formula>LEFT(C21,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C24">
-    <cfRule type="expression" dxfId="19" priority="22" stopIfTrue="1">
+    <cfRule type="expression" dxfId="25" priority="22" stopIfTrue="1">
       <formula>LEFT(C24,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C27:C29">
-    <cfRule type="expression" dxfId="18" priority="21" stopIfTrue="1">
+    <cfRule type="expression" dxfId="24" priority="21" stopIfTrue="1">
       <formula>LEFT(C27,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C42:C55">
-    <cfRule type="expression" dxfId="17" priority="20" stopIfTrue="1">
+    <cfRule type="expression" dxfId="23" priority="20" stopIfTrue="1">
       <formula>LEFT(C42,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C65">
-    <cfRule type="expression" dxfId="16" priority="19" stopIfTrue="1">
+    <cfRule type="expression" dxfId="22" priority="19" stopIfTrue="1">
       <formula>LEFT(C65,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C72">
-    <cfRule type="expression" dxfId="15" priority="18" stopIfTrue="1">
+    <cfRule type="expression" dxfId="21" priority="18" stopIfTrue="1">
       <formula>LEFT(C72,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C74">
-    <cfRule type="expression" dxfId="14" priority="17" stopIfTrue="1">
+    <cfRule type="expression" dxfId="20" priority="17" stopIfTrue="1">
       <formula>LEFT(C74,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C85">
-    <cfRule type="expression" dxfId="13" priority="15" stopIfTrue="1">
+    <cfRule type="expression" dxfId="19" priority="15" stopIfTrue="1">
       <formula>LEFT(C85,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C88:C92 C97">
-    <cfRule type="expression" dxfId="12" priority="14" stopIfTrue="1">
+    <cfRule type="expression" dxfId="18" priority="14" stopIfTrue="1">
       <formula>LEFT(C88,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C129:C133">
-    <cfRule type="expression" dxfId="11" priority="13" stopIfTrue="1">
-      <formula>LEFT(C129,LEN("#"))="#"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C135">
-    <cfRule type="expression" dxfId="10" priority="12" stopIfTrue="1">
-      <formula>LEFT(C135,LEN("#"))="#"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C137">
-    <cfRule type="expression" dxfId="9" priority="11" stopIfTrue="1">
+  <conditionalFormatting sqref="C137:C141">
+    <cfRule type="expression" dxfId="17" priority="13" stopIfTrue="1">
       <formula>LEFT(C137,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="C143">
+    <cfRule type="expression" dxfId="16" priority="12" stopIfTrue="1">
+      <formula>LEFT(C143,LEN("#"))="#"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="C145">
-    <cfRule type="expression" dxfId="8" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="15" priority="11" stopIfTrue="1">
       <formula>LEFT(C145,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C144">
-    <cfRule type="expression" dxfId="7" priority="9" stopIfTrue="1">
-      <formula>LEFT(C144,LEN("#"))="#"</formula>
+  <conditionalFormatting sqref="C153">
+    <cfRule type="expression" dxfId="14" priority="10" stopIfTrue="1">
+      <formula>LEFT(C153,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C149:C151">
-    <cfRule type="expression" dxfId="6" priority="8" stopIfTrue="1">
-      <formula>LEFT(C149,LEN("#"))="#"</formula>
+  <conditionalFormatting sqref="C152">
+    <cfRule type="expression" dxfId="13" priority="9" stopIfTrue="1">
+      <formula>LEFT(C152,LEN("#"))="#"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C157:C159">
+    <cfRule type="expression" dxfId="12" priority="8" stopIfTrue="1">
+      <formula>LEFT(C157,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C95">
-    <cfRule type="expression" dxfId="5" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="11" priority="7" stopIfTrue="1">
       <formula>LEFT(C95,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C96">
-    <cfRule type="expression" dxfId="4" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="10" priority="6" stopIfTrue="1">
       <formula>LEFT(C96,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C98">
-    <cfRule type="expression" dxfId="3" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="9" priority="5" stopIfTrue="1">
       <formula>LEFT(C98,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C99">
-    <cfRule type="expression" dxfId="2" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="8" priority="4" stopIfTrue="1">
       <formula>LEFT(C99,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C100">
-    <cfRule type="expression" dxfId="1" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="7" priority="3" stopIfTrue="1">
       <formula>LEFT(C100,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C93">
-    <cfRule type="expression" dxfId="0" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="6" priority="1" stopIfTrue="1">
       <formula>LEFT(C93,LEN("#"))="#"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3356,25 +3652,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement>
-    <Document_x0020_Subject xmlns="6c14b9a8-0cf3-4383-834f-1018380d8abf">Detailed Design</Document_x0020_Subject>
-    <_Status xmlns="http://schemas.microsoft.com/sharepoint/v3/fields">Not Started</_Status>
-    <Document_x0020_Category xmlns="6c14b9a8-0cf3-4383-834f-1018380d8abf">Development</Document_x0020_Category>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A328EC7CAE967C42BF4B34D61A06A4B5" ma:contentTypeVersion="6" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="edcd34646fceb0c4bcc9308538c5ed43">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="http://schemas.microsoft.com/sharepoint/v3/fields" xmlns:ns3="6c14b9a8-0cf3-4383-834f-1018380d8abf" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9deb4a6428fe92bbf1d3db187a263d42" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3/fields"/>
@@ -3489,31 +3766,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A766AC35-CC0B-4B7E-9290-4E442146633E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/fields"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="6c14b9a8-0cf3-4383-834f-1018380d8abf"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8B70E11A-8654-45A3-8334-FE029118DA1A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement>
+    <Document_x0020_Subject xmlns="6c14b9a8-0cf3-4383-834f-1018380d8abf">Detailed Design</Document_x0020_Subject>
+    <_Status xmlns="http://schemas.microsoft.com/sharepoint/v3/fields">Not Started</_Status>
+    <Document_x0020_Category xmlns="6c14b9a8-0cf3-4383-834f-1018380d8abf">Development</Document_x0020_Category>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4D694661-529E-46DF-82AC-97A5D29D95C8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3529,4 +3801,28 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/internal/2005/internalDocumentation"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8B70E11A-8654-45A3-8334-FE029118DA1A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A766AC35-CC0B-4B7E-9290-4E442146633E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/fields"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="6c14b9a8-0cf3-4383-834f-1018380d8abf"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>